<commit_message>
Updated a tonne of files and generated new graphs
Still need to do super fancy radial bar chart, which is less 'horionatally' challenged.
</commit_message>
<xml_diff>
--- a/SkillAnalysis_191201.xlsx
+++ b/SkillAnalysis_191201.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://heriotwatt-my.sharepoint.com/personal/cy11_hw_ac_uk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbee\Documents\github\rowenaIndustrialReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{FC1DA54A-6B94-43A8-A583-607BFB5B8DAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8B6CBBB1-9CDB-485F-93A5-973D56E44AC8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B1C38A-CFB0-4E66-949D-E19550D5F87A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="7" xr2:uid="{91381AA0-CDED-4A24-B704-028EFDFCCA12}"/>
   </bookViews>
@@ -30,7 +30,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="443">
   <si>
     <t>SM1i</t>
   </si>
@@ -1388,6 +1387,12 @@
   <si>
     <t>Interest</t>
   </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
 </sst>
 </file>
 
@@ -1396,7 +1401,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1543,6 +1548,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2257,7 +2270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="226">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2587,39 +2600,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2628,6 +2608,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
@@ -2644,15 +2627,53 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2977,13 +2998,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5495,7 +5509,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{874454D2-E7A1-49C7-B3D6-F4649E047457}" name="Table1" displayName="Table1" ref="E4:J46" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{874454D2-E7A1-49C7-B3D6-F4649E047457}" name="Table1" displayName="Table1" ref="E4:J46" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18">
   <autoFilter ref="E4:J46" xr:uid="{FEDCF0A9-C11D-4890-955E-26CD106F3055}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -5505,19 +5519,19 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{940E411E-8400-40B8-96F9-44DFEFD8B182}" name="Project Name" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{940E411E-8400-40B8-96F9-44DFEFD8B182}" name="Project Name" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{BDE580CA-F9F8-4D94-9E58-6003AEF4AA73}" name="Sector"/>
-    <tableColumn id="3" xr3:uid="{546043E9-4585-40C9-947B-FB0ACAAF1C1C}" name="RIBA Stage" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{546043E9-4585-40C9-947B-FB0ACAAF1C1C}" name="RIBA Stage" dataDxfId="16"/>
     <tableColumn id="4" xr3:uid="{76BAC2BF-66A2-4DE3-9C84-B30533F75941}" name="Responsibilites"/>
     <tableColumn id="5" xr3:uid="{FAC3E5BE-A627-47EF-842A-936B8C5C24E4}" name="Technical Level"/>
-    <tableColumn id="6" xr3:uid="{3C424575-28AB-4F48-860E-C6F0286F864B}" name="Technical Background" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{3C424575-28AB-4F48-860E-C6F0286F864B}" name="Technical Background" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BB18F5F7-94C3-412F-B41C-89A49D3A1B6E}" name="Table2" displayName="Table2" ref="E4:H14" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BB18F5F7-94C3-412F-B41C-89A49D3A1B6E}" name="Table2" displayName="Table2" ref="E4:H14" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="E4:H14" xr:uid="{AA3D3DA4-2083-490B-A96B-2B6A8C8A062C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -5525,17 +5539,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D8A65525-04C8-4BE8-8B00-98640AF74A25}" name="Date" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{B8AB7846-FFD4-480C-9E95-269BFDB4D83F}" name="Type" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{ACD4220A-1F09-4CA6-83C8-1ADE750BFEDF}" name="Organisation" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{14F76FFF-750E-4CE0-B5B1-C105AAD8B551}" name="Title" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{D8A65525-04C8-4BE8-8B00-98640AF74A25}" name="Date" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{B8AB7846-FFD4-480C-9E95-269BFDB4D83F}" name="Type" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{ACD4220A-1F09-4CA6-83C8-1ADE750BFEDF}" name="Organisation" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{14F76FFF-750E-4CE0-B5B1-C105AAD8B551}" name="Title" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99DCEDA8-FD6A-4E18-9BB2-84664FBDA263}" name="Table3" displayName="Table3" ref="E4:H23" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99DCEDA8-FD6A-4E18-9BB2-84664FBDA263}" name="Table3" displayName="Table3" ref="E4:H23" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="E4:H23" xr:uid="{E199B8BB-BC91-441E-9101-4AE76CC62D13}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -5543,10 +5557,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{590C04C5-5CDC-4ECD-B6EA-7E8890540C41}" name="Date" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{3498CE5B-8610-4066-A61D-90644C3BD461}" name="Type" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{2AD8B7EA-1272-40CF-AABF-BACD4051D629}" name="Title" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{3D9453BF-042C-4CB9-B176-9466A2A70913}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{590C04C5-5CDC-4ECD-B6EA-7E8890540C41}" name="Date" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{3498CE5B-8610-4066-A61D-90644C3BD461}" name="Type" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{2AD8B7EA-1272-40CF-AABF-BACD4051D629}" name="Title" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{3D9453BF-042C-4CB9-B176-9466A2A70913}" name="Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5857,22 +5871,22 @@
       <selection pane="bottomLeft" activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.26953125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="5.1328125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="5.953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="6" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47" style="10" customWidth="1"/>
-    <col min="5" max="5" width="4.1796875" customWidth="1"/>
-    <col min="6" max="12" width="4.5" customWidth="1"/>
-    <col min="13" max="13" width="4.31640625" customWidth="1"/>
-    <col min="14" max="44" width="4.5" customWidth="1"/>
-    <col min="45" max="45" width="3.86328125" customWidth="1"/>
-    <col min="46" max="54" width="4.1328125" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" customWidth="1"/>
+    <col min="6" max="12" width="4.42578125" customWidth="1"/>
+    <col min="13" max="13" width="4.28515625" customWidth="1"/>
+    <col min="14" max="44" width="4.42578125" customWidth="1"/>
+    <col min="45" max="45" width="3.85546875" customWidth="1"/>
+    <col min="46" max="54" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" ht="16.5" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="2" spans="1:79" s="27" customFormat="1" ht="196.25" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:79" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:79" s="27" customFormat="1" ht="198" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="14"/>
       <c r="C2" s="13"/>
@@ -6047,72 +6061,72 @@
       <c r="BZ2" s="25"/>
       <c r="CA2" s="26"/>
     </row>
-    <row r="3" spans="1:79" s="2" customFormat="1" ht="18.5" x14ac:dyDescent="0.9">
+    <row r="3" spans="1:79" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
       <c r="D3" s="12"/>
-      <c r="E3" s="213" t="s">
+      <c r="E3" s="223" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="213"/>
-      <c r="G3" s="213"/>
-      <c r="H3" s="213"/>
-      <c r="I3" s="213"/>
-      <c r="J3" s="213"/>
-      <c r="K3" s="213"/>
-      <c r="L3" s="213"/>
-      <c r="M3" s="209" t="s">
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="223"/>
+      <c r="I3" s="223"/>
+      <c r="J3" s="223"/>
+      <c r="K3" s="223"/>
+      <c r="L3" s="223"/>
+      <c r="M3" s="220" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="209"/>
-      <c r="O3" s="209"/>
-      <c r="P3" s="209"/>
-      <c r="Q3" s="209"/>
-      <c r="R3" s="209"/>
-      <c r="S3" s="209"/>
-      <c r="T3" s="209"/>
-      <c r="U3" s="210" t="s">
+      <c r="N3" s="220"/>
+      <c r="O3" s="220"/>
+      <c r="P3" s="220"/>
+      <c r="Q3" s="220"/>
+      <c r="R3" s="220"/>
+      <c r="S3" s="220"/>
+      <c r="T3" s="220"/>
+      <c r="U3" s="221" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="210"/>
-      <c r="W3" s="210"/>
-      <c r="X3" s="210"/>
-      <c r="Y3" s="210"/>
-      <c r="Z3" s="210"/>
-      <c r="AA3" s="210"/>
-      <c r="AB3" s="210"/>
-      <c r="AC3" s="211" t="s">
+      <c r="V3" s="221"/>
+      <c r="W3" s="221"/>
+      <c r="X3" s="221"/>
+      <c r="Y3" s="221"/>
+      <c r="Z3" s="221"/>
+      <c r="AA3" s="221"/>
+      <c r="AB3" s="221"/>
+      <c r="AC3" s="222" t="s">
         <v>21</v>
       </c>
-      <c r="AD3" s="211"/>
-      <c r="AE3" s="211"/>
-      <c r="AF3" s="211"/>
-      <c r="AG3" s="211"/>
-      <c r="AH3" s="220" t="s">
+      <c r="AD3" s="222"/>
+      <c r="AE3" s="222"/>
+      <c r="AF3" s="222"/>
+      <c r="AG3" s="222"/>
+      <c r="AH3" s="210" t="s">
         <v>22</v>
       </c>
-      <c r="AI3" s="220"/>
-      <c r="AJ3" s="220"/>
-      <c r="AK3" s="220"/>
-      <c r="AL3" s="220"/>
-      <c r="AM3" s="220"/>
-      <c r="AN3" s="220"/>
-      <c r="AO3" s="221" t="s">
+      <c r="AI3" s="210"/>
+      <c r="AJ3" s="210"/>
+      <c r="AK3" s="210"/>
+      <c r="AL3" s="210"/>
+      <c r="AM3" s="210"/>
+      <c r="AN3" s="210"/>
+      <c r="AO3" s="211" t="s">
         <v>153</v>
       </c>
-      <c r="AP3" s="222"/>
-      <c r="AQ3" s="222"/>
-      <c r="AR3" s="222"/>
-      <c r="AS3" s="222"/>
-      <c r="AT3" s="222"/>
-      <c r="AU3" s="223"/>
-      <c r="AV3" s="216" t="s">
+      <c r="AP3" s="212"/>
+      <c r="AQ3" s="212"/>
+      <c r="AR3" s="212"/>
+      <c r="AS3" s="212"/>
+      <c r="AT3" s="212"/>
+      <c r="AU3" s="213"/>
+      <c r="AV3" s="205" t="s">
         <v>250</v>
       </c>
-      <c r="AW3" s="217"/>
-      <c r="AX3" s="217"/>
-      <c r="AY3" s="218"/>
+      <c r="AW3" s="206"/>
+      <c r="AX3" s="206"/>
+      <c r="AY3" s="207"/>
       <c r="AZ3" s="1"/>
       <c r="BA3" s="1"/>
       <c r="BB3" s="1"/>
@@ -6142,11 +6156,11 @@
       <c r="BZ3" s="1"/>
       <c r="CA3" s="4"/>
     </row>
-    <row r="4" spans="1:79" ht="32.4" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="205" t="s">
+    <row r="4" spans="1:79" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="217" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="212" t="s">
+      <c r="B4" s="215" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="15" t="s">
@@ -6267,9 +6281,9 @@
       <c r="BH4" s="41"/>
       <c r="BI4" s="41"/>
     </row>
-    <row r="5" spans="1:79" ht="81" x14ac:dyDescent="0.75">
-      <c r="A5" s="206"/>
-      <c r="B5" s="212"/>
+    <row r="5" spans="1:79" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="218"/>
+      <c r="B5" s="215"/>
       <c r="C5" s="15" t="s">
         <v>1</v>
       </c>
@@ -6370,9 +6384,9 @@
       <c r="BH5" s="41"/>
       <c r="BI5" s="41"/>
     </row>
-    <row r="6" spans="1:79" ht="116.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A6" s="206"/>
-      <c r="B6" s="212"/>
+    <row r="6" spans="1:79" ht="116.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="218"/>
+      <c r="B6" s="215"/>
       <c r="C6" s="42" t="s">
         <v>2</v>
       </c>
@@ -6445,9 +6459,9 @@
       <c r="BH6" s="47"/>
       <c r="BI6" s="47"/>
     </row>
-    <row r="7" spans="1:79" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A7" s="206"/>
-      <c r="B7" s="212" t="s">
+    <row r="7" spans="1:79" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="218"/>
+      <c r="B7" s="215" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="38" t="s">
@@ -6560,9 +6574,9 @@
       <c r="BH7" s="50"/>
       <c r="BI7" s="50"/>
     </row>
-    <row r="8" spans="1:79" ht="81" x14ac:dyDescent="0.75">
-      <c r="A8" s="206"/>
-      <c r="B8" s="212"/>
+    <row r="8" spans="1:79" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="218"/>
+      <c r="B8" s="215"/>
       <c r="C8" s="15" t="s">
         <v>4</v>
       </c>
@@ -6651,9 +6665,9 @@
       <c r="BH8" s="41"/>
       <c r="BI8" s="41"/>
     </row>
-    <row r="9" spans="1:79" ht="81" x14ac:dyDescent="0.75">
-      <c r="A9" s="206"/>
-      <c r="B9" s="212"/>
+    <row r="9" spans="1:79" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="218"/>
+      <c r="B9" s="215"/>
       <c r="C9" s="15" t="s">
         <v>5</v>
       </c>
@@ -6724,9 +6738,9 @@
       <c r="BH9" s="47"/>
       <c r="BI9" s="47"/>
     </row>
-    <row r="10" spans="1:79" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A10" s="206"/>
-      <c r="B10" s="212" t="s">
+    <row r="10" spans="1:79" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="218"/>
+      <c r="B10" s="215" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -6817,9 +6831,9 @@
       <c r="BH10" s="50"/>
       <c r="BI10" s="50"/>
     </row>
-    <row r="11" spans="1:79" ht="54" x14ac:dyDescent="0.75">
-      <c r="A11" s="206"/>
-      <c r="B11" s="212"/>
+    <row r="11" spans="1:79" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="218"/>
+      <c r="B11" s="215"/>
       <c r="C11" s="15" t="s">
         <v>7</v>
       </c>
@@ -6896,8 +6910,8 @@
       <c r="BH11" s="47"/>
       <c r="BI11" s="47"/>
     </row>
-    <row r="12" spans="1:79" ht="27" x14ac:dyDescent="0.75">
-      <c r="A12" s="206"/>
+    <row r="12" spans="1:79" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="218"/>
       <c r="B12" s="17" t="s">
         <v>14</v>
       </c>
@@ -6999,8 +7013,8 @@
       <c r="BH12" s="56"/>
       <c r="BI12" s="56"/>
     </row>
-    <row r="13" spans="1:79" ht="54" x14ac:dyDescent="0.75">
-      <c r="A13" s="206"/>
+    <row r="13" spans="1:79" ht="51" x14ac:dyDescent="0.25">
+      <c r="A13" s="218"/>
       <c r="B13" s="17" t="s">
         <v>15</v>
       </c>
@@ -7076,8 +7090,8 @@
       <c r="BH13" s="56"/>
       <c r="BI13" s="56"/>
     </row>
-    <row r="14" spans="1:79" ht="54" x14ac:dyDescent="0.75">
-      <c r="A14" s="207"/>
+    <row r="14" spans="1:79" ht="51" x14ac:dyDescent="0.25">
+      <c r="A14" s="219"/>
       <c r="B14" s="17" t="s">
         <v>16</v>
       </c>
@@ -7185,8 +7199,8 @@
       <c r="BH14" s="56"/>
       <c r="BI14" s="56"/>
     </row>
-    <row r="15" spans="1:79" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A15" s="215" t="s">
+    <row r="15" spans="1:79" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="214" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="208" t="s">
@@ -7270,8 +7284,8 @@
       <c r="BH15" s="50"/>
       <c r="BI15" s="50"/>
     </row>
-    <row r="16" spans="1:79" ht="27" x14ac:dyDescent="0.75">
-      <c r="A16" s="215"/>
+    <row r="16" spans="1:79" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="214"/>
       <c r="B16" s="208"/>
       <c r="C16" s="15" t="s">
         <v>24</v>
@@ -7371,8 +7385,8 @@
       <c r="BH16" s="41"/>
       <c r="BI16" s="41"/>
     </row>
-    <row r="17" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A17" s="215"/>
+    <row r="17" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="214"/>
       <c r="B17" s="208"/>
       <c r="C17" s="15" t="s">
         <v>25</v>
@@ -7450,9 +7464,9 @@
       <c r="BH17" s="47"/>
       <c r="BI17" s="47"/>
     </row>
-    <row r="18" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A18" s="215"/>
-      <c r="B18" s="214" t="s">
+    <row r="18" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="214"/>
+      <c r="B18" s="216" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="15" t="s">
@@ -7535,9 +7549,9 @@
       <c r="BH18" s="50"/>
       <c r="BI18" s="50"/>
     </row>
-    <row r="19" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A19" s="215"/>
-      <c r="B19" s="214"/>
+    <row r="19" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="214"/>
+      <c r="B19" s="216"/>
       <c r="C19" s="15" t="s">
         <v>27</v>
       </c>
@@ -7612,9 +7626,9 @@
       <c r="BH19" s="47"/>
       <c r="BI19" s="47"/>
     </row>
-    <row r="20" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A20" s="215"/>
-      <c r="B20" s="212" t="s">
+    <row r="20" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="214"/>
+      <c r="B20" s="215" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="15" t="s">
@@ -7705,9 +7719,9 @@
       <c r="BH20" s="50"/>
       <c r="BI20" s="50"/>
     </row>
-    <row r="21" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A21" s="215"/>
-      <c r="B21" s="212"/>
+    <row r="21" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="214"/>
+      <c r="B21" s="215"/>
       <c r="C21" s="15" t="s">
         <v>29</v>
       </c>
@@ -7786,9 +7800,9 @@
       <c r="BH21" s="41"/>
       <c r="BI21" s="41"/>
     </row>
-    <row r="22" spans="1:61" ht="54" x14ac:dyDescent="0.75">
-      <c r="A22" s="215"/>
-      <c r="B22" s="212"/>
+    <row r="22" spans="1:61" ht="51" x14ac:dyDescent="0.25">
+      <c r="A22" s="214"/>
+      <c r="B22" s="215"/>
       <c r="C22" s="15" t="s">
         <v>30</v>
       </c>
@@ -7861,9 +7875,9 @@
       <c r="BH22" s="47"/>
       <c r="BI22" s="47"/>
     </row>
-    <row r="23" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A23" s="215"/>
-      <c r="B23" s="212" t="s">
+    <row r="23" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="214"/>
+      <c r="B23" s="215" t="s">
         <v>38</v>
       </c>
       <c r="C23" s="15" t="s">
@@ -7950,9 +7964,9 @@
       <c r="BH23" s="50"/>
       <c r="BI23" s="50"/>
     </row>
-    <row r="24" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A24" s="215"/>
-      <c r="B24" s="212"/>
+    <row r="24" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="214"/>
+      <c r="B24" s="215"/>
       <c r="C24" s="15" t="s">
         <v>32</v>
       </c>
@@ -8029,9 +8043,9 @@
       <c r="BH24" s="41"/>
       <c r="BI24" s="41"/>
     </row>
-    <row r="25" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A25" s="215"/>
-      <c r="B25" s="212"/>
+    <row r="25" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="214"/>
+      <c r="B25" s="215"/>
       <c r="C25" s="15" t="s">
         <v>33</v>
       </c>
@@ -8102,8 +8116,8 @@
       <c r="BH25" s="47"/>
       <c r="BI25" s="47"/>
     </row>
-    <row r="26" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A26" s="215"/>
+    <row r="26" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="214"/>
       <c r="B26" s="18" t="s">
         <v>39</v>
       </c>
@@ -8191,8 +8205,8 @@
       <c r="BH26" s="56"/>
       <c r="BI26" s="56"/>
     </row>
-    <row r="27" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A27" s="215"/>
+    <row r="27" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="214"/>
       <c r="B27" s="18" t="s">
         <v>40</v>
       </c>
@@ -8276,11 +8290,11 @@
       <c r="BH27" s="56"/>
       <c r="BI27" s="56"/>
     </row>
-    <row r="28" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A28" s="215" t="s">
+    <row r="28" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="214" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="212" t="s">
+      <c r="B28" s="215" t="s">
         <v>43</v>
       </c>
       <c r="C28" s="15" t="s">
@@ -8379,9 +8393,9 @@
       <c r="BH28" s="50"/>
       <c r="BI28" s="50"/>
     </row>
-    <row r="29" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A29" s="215"/>
-      <c r="B29" s="212"/>
+    <row r="29" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="214"/>
+      <c r="B29" s="215"/>
       <c r="C29" s="15" t="s">
         <v>43</v>
       </c>
@@ -8452,9 +8466,9 @@
       <c r="BH29" s="47"/>
       <c r="BI29" s="47"/>
     </row>
-    <row r="30" spans="1:61" ht="54" x14ac:dyDescent="0.75">
-      <c r="A30" s="215"/>
-      <c r="B30" s="212" t="s">
+    <row r="30" spans="1:61" ht="51" x14ac:dyDescent="0.25">
+      <c r="A30" s="214"/>
+      <c r="B30" s="215" t="s">
         <v>45</v>
       </c>
       <c r="C30" s="15" t="s">
@@ -8549,9 +8563,9 @@
       <c r="BH30" s="50"/>
       <c r="BI30" s="50"/>
     </row>
-    <row r="31" spans="1:61" ht="54" x14ac:dyDescent="0.75">
-      <c r="A31" s="215"/>
-      <c r="B31" s="212"/>
+    <row r="31" spans="1:61" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="214"/>
+      <c r="B31" s="215"/>
       <c r="C31" s="15" t="s">
         <v>45</v>
       </c>
@@ -8630,9 +8644,9 @@
       <c r="BH31" s="47"/>
       <c r="BI31" s="47"/>
     </row>
-    <row r="32" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A32" s="215"/>
-      <c r="B32" s="212" t="s">
+    <row r="32" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="214"/>
+      <c r="B32" s="215" t="s">
         <v>46</v>
       </c>
       <c r="C32" s="15" t="s">
@@ -8713,9 +8727,9 @@
       <c r="BH32" s="50"/>
       <c r="BI32" s="50"/>
     </row>
-    <row r="33" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A33" s="215"/>
-      <c r="B33" s="212"/>
+    <row r="33" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="214"/>
+      <c r="B33" s="215"/>
       <c r="C33" s="15" t="s">
         <v>47</v>
       </c>
@@ -8782,9 +8796,9 @@
       <c r="BH33" s="41"/>
       <c r="BI33" s="41"/>
     </row>
-    <row r="34" spans="1:61" ht="54" x14ac:dyDescent="0.75">
-      <c r="A34" s="215"/>
-      <c r="B34" s="212"/>
+    <row r="34" spans="1:61" ht="51" x14ac:dyDescent="0.25">
+      <c r="A34" s="214"/>
+      <c r="B34" s="215"/>
       <c r="C34" s="15" t="s">
         <v>48</v>
       </c>
@@ -8849,9 +8863,9 @@
       <c r="BH34" s="47"/>
       <c r="BI34" s="47"/>
     </row>
-    <row r="35" spans="1:61" ht="54" x14ac:dyDescent="0.75">
-      <c r="A35" s="215"/>
-      <c r="B35" s="212" t="s">
+    <row r="35" spans="1:61" ht="51" x14ac:dyDescent="0.25">
+      <c r="A35" s="214"/>
+      <c r="B35" s="215" t="s">
         <v>50</v>
       </c>
       <c r="C35" s="15" t="s">
@@ -8944,9 +8958,9 @@
       <c r="BH35" s="50"/>
       <c r="BI35" s="50"/>
     </row>
-    <row r="36" spans="1:61" ht="67.5" x14ac:dyDescent="0.75">
-      <c r="A36" s="215"/>
-      <c r="B36" s="212"/>
+    <row r="36" spans="1:61" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="214"/>
+      <c r="B36" s="215"/>
       <c r="C36" s="15" t="s">
         <v>50</v>
       </c>
@@ -9017,9 +9031,9 @@
       <c r="BH36" s="47"/>
       <c r="BI36" s="47"/>
     </row>
-    <row r="37" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A37" s="215"/>
-      <c r="B37" s="212" t="s">
+    <row r="37" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="214"/>
+      <c r="B37" s="215" t="s">
         <v>52</v>
       </c>
       <c r="C37" s="15" t="s">
@@ -9094,9 +9108,9 @@
       <c r="BH37" s="50"/>
       <c r="BI37" s="50"/>
     </row>
-    <row r="38" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A38" s="215"/>
-      <c r="B38" s="212"/>
+    <row r="38" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="214"/>
+      <c r="B38" s="215"/>
       <c r="C38" s="15" t="s">
         <v>52</v>
       </c>
@@ -9163,8 +9177,8 @@
       <c r="BH38" s="47"/>
       <c r="BI38" s="47"/>
     </row>
-    <row r="39" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A39" s="215"/>
+    <row r="39" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="214"/>
       <c r="B39" s="18" t="s">
         <v>53</v>
       </c>
@@ -9250,8 +9264,8 @@
       <c r="BH39" s="56"/>
       <c r="BI39" s="56"/>
     </row>
-    <row r="40" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A40" s="215"/>
+    <row r="40" spans="1:61" ht="51" x14ac:dyDescent="0.25">
+      <c r="A40" s="214"/>
       <c r="B40" s="18" t="s">
         <v>56</v>
       </c>
@@ -9331,8 +9345,8 @@
       <c r="BH40" s="56"/>
       <c r="BI40" s="56"/>
     </row>
-    <row r="41" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A41" s="215"/>
+    <row r="41" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="214"/>
       <c r="B41" s="18" t="s">
         <v>57</v>
       </c>
@@ -9412,11 +9426,11 @@
       <c r="BH41" s="56"/>
       <c r="BI41" s="56"/>
     </row>
-    <row r="42" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A42" s="215" t="s">
+    <row r="42" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="214" t="s">
         <v>76</v>
       </c>
-      <c r="B42" s="212" t="s">
+      <c r="B42" s="215" t="s">
         <v>59</v>
       </c>
       <c r="C42" s="15" t="s">
@@ -9503,9 +9517,9 @@
       <c r="BH42" s="50"/>
       <c r="BI42" s="50"/>
     </row>
-    <row r="43" spans="1:61" ht="54" x14ac:dyDescent="0.75">
-      <c r="A43" s="215"/>
-      <c r="B43" s="212"/>
+    <row r="43" spans="1:61" ht="51" x14ac:dyDescent="0.25">
+      <c r="A43" s="214"/>
+      <c r="B43" s="215"/>
       <c r="C43" s="15" t="s">
         <v>60</v>
       </c>
@@ -9590,8 +9604,8 @@
       <c r="BH43" s="47"/>
       <c r="BI43" s="47"/>
     </row>
-    <row r="44" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A44" s="215"/>
+    <row r="44" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="214"/>
       <c r="B44" s="18" t="s">
         <v>61</v>
       </c>
@@ -9675,8 +9689,8 @@
       <c r="BH44" s="56"/>
       <c r="BI44" s="56"/>
     </row>
-    <row r="45" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A45" s="215"/>
+    <row r="45" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="214"/>
       <c r="B45" s="208" t="s">
         <v>72</v>
       </c>
@@ -9762,8 +9776,8 @@
       <c r="BH45" s="50"/>
       <c r="BI45" s="50"/>
     </row>
-    <row r="46" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A46" s="215"/>
+    <row r="46" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="214"/>
       <c r="B46" s="208"/>
       <c r="C46" s="15" t="s">
         <v>63</v>
@@ -9835,8 +9849,8 @@
       <c r="BH46" s="41"/>
       <c r="BI46" s="41"/>
     </row>
-    <row r="47" spans="1:61" ht="54" x14ac:dyDescent="0.75">
-      <c r="A47" s="215"/>
+    <row r="47" spans="1:61" ht="51" x14ac:dyDescent="0.25">
+      <c r="A47" s="214"/>
       <c r="B47" s="208"/>
       <c r="C47" s="15" t="s">
         <v>64</v>
@@ -9902,8 +9916,8 @@
       <c r="BH47" s="47"/>
       <c r="BI47" s="47"/>
     </row>
-    <row r="48" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A48" s="215"/>
+    <row r="48" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="214"/>
       <c r="B48" s="208" t="s">
         <v>73</v>
       </c>
@@ -10007,8 +10021,8 @@
       <c r="BH48" s="50"/>
       <c r="BI48" s="50"/>
     </row>
-    <row r="49" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A49" s="215"/>
+    <row r="49" spans="1:61" ht="51" x14ac:dyDescent="0.25">
+      <c r="A49" s="214"/>
       <c r="B49" s="208"/>
       <c r="C49" s="15" t="s">
         <v>66</v>
@@ -10088,8 +10102,8 @@
       <c r="BH49" s="47"/>
       <c r="BI49" s="47"/>
     </row>
-    <row r="50" spans="1:61" ht="54" x14ac:dyDescent="0.75">
-      <c r="A50" s="215"/>
+    <row r="50" spans="1:61" ht="51" x14ac:dyDescent="0.25">
+      <c r="A50" s="214"/>
       <c r="B50" s="208" t="s">
         <v>67</v>
       </c>
@@ -10177,8 +10191,8 @@
       <c r="BH50" s="50"/>
       <c r="BI50" s="50"/>
     </row>
-    <row r="51" spans="1:61" ht="67.5" x14ac:dyDescent="0.75">
-      <c r="A51" s="215"/>
+    <row r="51" spans="1:61" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="214"/>
       <c r="B51" s="208"/>
       <c r="C51" s="15" t="s">
         <v>68</v>
@@ -10256,8 +10270,8 @@
       <c r="BH51" s="47"/>
       <c r="BI51" s="47"/>
     </row>
-    <row r="52" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A52" s="215"/>
+    <row r="52" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="214"/>
       <c r="B52" s="208" t="s">
         <v>74</v>
       </c>
@@ -10349,8 +10363,8 @@
       <c r="BH52" s="50"/>
       <c r="BI52" s="50"/>
     </row>
-    <row r="53" spans="1:61" ht="47.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A53" s="215"/>
+    <row r="53" spans="1:61" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="214"/>
       <c r="B53" s="208"/>
       <c r="C53" s="15" t="s">
         <v>201</v>
@@ -10426,8 +10440,8 @@
       <c r="BH53" s="41"/>
       <c r="BI53" s="41"/>
     </row>
-    <row r="54" spans="1:61" ht="54" x14ac:dyDescent="0.75">
-      <c r="A54" s="215"/>
+    <row r="54" spans="1:61" ht="51" x14ac:dyDescent="0.25">
+      <c r="A54" s="214"/>
       <c r="B54" s="208"/>
       <c r="C54" s="15" t="s">
         <v>70</v>
@@ -10493,8 +10507,8 @@
       <c r="BH54" s="47"/>
       <c r="BI54" s="47"/>
     </row>
-    <row r="55" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A55" s="215"/>
+    <row r="55" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A55" s="214"/>
       <c r="B55" s="17" t="s">
         <v>75</v>
       </c>
@@ -10570,8 +10584,8 @@
       <c r="BH55" s="56"/>
       <c r="BI55" s="56"/>
     </row>
-    <row r="56" spans="1:61" ht="48" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A56" s="215" t="s">
+    <row r="56" spans="1:61" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="214" t="s">
         <v>102</v>
       </c>
       <c r="B56" s="208" t="s">
@@ -10683,8 +10697,8 @@
       <c r="BH56" s="50"/>
       <c r="BI56" s="50"/>
     </row>
-    <row r="57" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A57" s="215"/>
+    <row r="57" spans="1:61" ht="51" x14ac:dyDescent="0.25">
+      <c r="A57" s="214"/>
       <c r="B57" s="208"/>
       <c r="C57" s="15" t="s">
         <v>78</v>
@@ -10782,8 +10796,8 @@
       <c r="BH57" s="47"/>
       <c r="BI57" s="47"/>
     </row>
-    <row r="58" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A58" s="215"/>
+    <row r="58" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="214"/>
       <c r="B58" s="208" t="s">
         <v>96</v>
       </c>
@@ -10887,8 +10901,8 @@
       <c r="BH58" s="50"/>
       <c r="BI58" s="50"/>
     </row>
-    <row r="59" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A59" s="215"/>
+    <row r="59" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="214"/>
       <c r="B59" s="208"/>
       <c r="C59" s="15" t="s">
         <v>80</v>
@@ -10974,8 +10988,8 @@
       <c r="BH59" s="41"/>
       <c r="BI59" s="41"/>
     </row>
-    <row r="60" spans="1:61" ht="54" x14ac:dyDescent="0.75">
-      <c r="A60" s="215"/>
+    <row r="60" spans="1:61" ht="51" x14ac:dyDescent="0.25">
+      <c r="A60" s="214"/>
       <c r="B60" s="208"/>
       <c r="C60" s="15" t="s">
         <v>81</v>
@@ -11041,8 +11055,8 @@
       <c r="BH60" s="47"/>
       <c r="BI60" s="47"/>
     </row>
-    <row r="61" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A61" s="215"/>
+    <row r="61" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="214"/>
       <c r="B61" s="208" t="s">
         <v>97</v>
       </c>
@@ -11126,8 +11140,8 @@
       <c r="BH61" s="50"/>
       <c r="BI61" s="50"/>
     </row>
-    <row r="62" spans="1:61" x14ac:dyDescent="0.75">
-      <c r="A62" s="215"/>
+    <row r="62" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A62" s="214"/>
       <c r="B62" s="208"/>
       <c r="C62" s="15" t="s">
         <v>210</v>
@@ -11205,8 +11219,8 @@
       <c r="BH62" s="47"/>
       <c r="BI62" s="47"/>
     </row>
-    <row r="63" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A63" s="215"/>
+    <row r="63" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="214"/>
       <c r="B63" s="208" t="s">
         <v>98</v>
       </c>
@@ -11308,8 +11322,8 @@
       <c r="BH63" s="50"/>
       <c r="BI63" s="50"/>
     </row>
-    <row r="64" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A64" s="215"/>
+    <row r="64" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A64" s="214"/>
       <c r="B64" s="208"/>
       <c r="C64" s="15" t="s">
         <v>98</v>
@@ -11393,8 +11407,8 @@
       <c r="BH64" s="41"/>
       <c r="BI64" s="41"/>
     </row>
-    <row r="65" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A65" s="215"/>
+    <row r="65" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="214"/>
       <c r="B65" s="208"/>
       <c r="C65" s="147" t="s">
         <v>84</v>
@@ -11478,8 +11492,8 @@
       <c r="BH65" s="47"/>
       <c r="BI65" s="47"/>
     </row>
-    <row r="66" spans="1:61" x14ac:dyDescent="0.75">
-      <c r="A66" s="215"/>
+    <row r="66" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A66" s="214"/>
       <c r="B66" s="17" t="s">
         <v>85</v>
       </c>
@@ -11559,8 +11573,8 @@
       <c r="BH66" s="56"/>
       <c r="BI66" s="56"/>
     </row>
-    <row r="67" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A67" s="215"/>
+    <row r="67" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="214"/>
       <c r="B67" s="208" t="s">
         <v>99</v>
       </c>
@@ -11654,8 +11668,8 @@
       <c r="BH67" s="50"/>
       <c r="BI67" s="50"/>
     </row>
-    <row r="68" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A68" s="215"/>
+    <row r="68" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A68" s="214"/>
       <c r="B68" s="208"/>
       <c r="C68" s="15" t="s">
         <v>87</v>
@@ -11733,8 +11747,8 @@
       <c r="BH68" s="47"/>
       <c r="BI68" s="47"/>
     </row>
-    <row r="69" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A69" s="215"/>
+    <row r="69" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="214"/>
       <c r="B69" s="17" t="s">
         <v>88</v>
       </c>
@@ -11812,8 +11826,8 @@
       <c r="BH69" s="56"/>
       <c r="BI69" s="56"/>
     </row>
-    <row r="70" spans="1:61" x14ac:dyDescent="0.75">
-      <c r="A70" s="215"/>
+    <row r="70" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A70" s="214"/>
       <c r="B70" s="17" t="s">
         <v>89</v>
       </c>
@@ -11901,8 +11915,8 @@
       <c r="BH70" s="56"/>
       <c r="BI70" s="56"/>
     </row>
-    <row r="71" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A71" s="215"/>
+    <row r="71" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A71" s="214"/>
       <c r="B71" s="17" t="s">
         <v>100</v>
       </c>
@@ -11986,8 +12000,8 @@
       <c r="BH71" s="56"/>
       <c r="BI71" s="56"/>
     </row>
-    <row r="72" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A72" s="215"/>
+    <row r="72" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="214"/>
       <c r="B72" s="17" t="s">
         <v>101</v>
       </c>
@@ -12063,8 +12077,8 @@
       <c r="BH72" s="56"/>
       <c r="BI72" s="56"/>
     </row>
-    <row r="73" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A73" s="215"/>
+    <row r="73" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="214"/>
       <c r="B73" s="208" t="s">
         <v>92</v>
       </c>
@@ -12148,8 +12162,8 @@
       <c r="BH73" s="50"/>
       <c r="BI73" s="50"/>
     </row>
-    <row r="74" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A74" s="215"/>
+    <row r="74" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="214"/>
       <c r="B74" s="208"/>
       <c r="C74" s="15" t="s">
         <v>92</v>
@@ -12229,8 +12243,8 @@
       <c r="BH74" s="41"/>
       <c r="BI74" s="41"/>
     </row>
-    <row r="75" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A75" s="215"/>
+    <row r="75" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A75" s="214"/>
       <c r="B75" s="208"/>
       <c r="C75" s="15" t="s">
         <v>94</v>
@@ -12308,8 +12322,8 @@
       <c r="BH75" s="47"/>
       <c r="BI75" s="47"/>
     </row>
-    <row r="76" spans="1:61" ht="40.5" x14ac:dyDescent="0.75">
-      <c r="A76" s="219" t="s">
+    <row r="76" spans="1:61" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A76" s="209" t="s">
         <v>111</v>
       </c>
       <c r="B76" s="17" t="s">
@@ -12421,8 +12435,8 @@
       <c r="BH76" s="56"/>
       <c r="BI76" s="56"/>
     </row>
-    <row r="77" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A77" s="219"/>
+    <row r="77" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="209"/>
       <c r="B77" s="17" t="s">
         <v>104</v>
       </c>
@@ -12520,8 +12534,8 @@
       <c r="BH77" s="56"/>
       <c r="BI77" s="56"/>
     </row>
-    <row r="78" spans="1:61" x14ac:dyDescent="0.75">
-      <c r="A78" s="219"/>
+    <row r="78" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A78" s="209"/>
       <c r="B78" s="208" t="s">
         <v>110</v>
       </c>
@@ -12641,8 +12655,8 @@
       <c r="BH78" s="50"/>
       <c r="BI78" s="50"/>
     </row>
-    <row r="79" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A79" s="219"/>
+    <row r="79" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="209"/>
       <c r="B79" s="208"/>
       <c r="C79" s="15" t="s">
         <v>107</v>
@@ -12748,8 +12762,8 @@
       <c r="BH79" s="41"/>
       <c r="BI79" s="41"/>
     </row>
-    <row r="80" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A80" s="219"/>
+    <row r="80" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A80" s="209"/>
       <c r="B80" s="208"/>
       <c r="C80" s="15" t="s">
         <v>108</v>
@@ -12825,8 +12839,8 @@
       <c r="BH80" s="47"/>
       <c r="BI80" s="47"/>
     </row>
-    <row r="81" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A81" s="219"/>
+    <row r="81" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A81" s="209"/>
       <c r="B81" s="208" t="s">
         <v>109</v>
       </c>
@@ -12926,8 +12940,8 @@
       <c r="BH81" s="50"/>
       <c r="BI81" s="50"/>
     </row>
-    <row r="82" spans="1:61" ht="27" x14ac:dyDescent="0.75">
-      <c r="A82" s="219"/>
+    <row r="82" spans="1:61" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A82" s="209"/>
       <c r="B82" s="208"/>
       <c r="C82" s="15" t="s">
         <v>109</v>
@@ -13011,12 +13025,34 @@
       <c r="BH82" s="47"/>
       <c r="BI82" s="47"/>
     </row>
-    <row r="86" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:61" x14ac:dyDescent="0.25">
       <c r="C86" s="15"/>
       <c r="D86" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="M3:T3"/>
+    <mergeCell ref="U3:AB3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="E3:L3"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A15:A27"/>
+    <mergeCell ref="A4:A14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A42:A55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A28:A41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B30:B31"/>
     <mergeCell ref="AV3:AY3"/>
     <mergeCell ref="B78:B80"/>
     <mergeCell ref="B81:B82"/>
@@ -13033,28 +13069,6 @@
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="B52:B54"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A42:A55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A28:A41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A15:A27"/>
-    <mergeCell ref="A4:A14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="M3:T3"/>
-    <mergeCell ref="U3:AB3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="E3:L3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="E4:AY14">
@@ -13118,12 +13132,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AY54 E56:AY82 E55:AN55 AP55:AY55">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </oddHeader>
+    <oddFooter xml:space="preserve">&amp;C      </oddFooter>
+    <evenHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </evenHeader>
+    <evenFooter xml:space="preserve">&amp;C      </evenFooter>
+    <firstHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </firstHeader>
+    <firstFooter xml:space="preserve">&amp;C      </firstFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -13135,14 +13157,14 @@
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.7265625" customWidth="1"/>
-    <col min="6" max="6" width="41.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>231</v>
       </c>
@@ -13150,7 +13172,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>233</v>
       </c>
@@ -13158,7 +13180,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>232</v>
       </c>
@@ -13166,7 +13188,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>234</v>
       </c>
@@ -13174,7 +13196,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>235</v>
       </c>
@@ -13182,7 +13204,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>236</v>
       </c>
@@ -13190,8 +13212,8 @@
         <v>241</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
-    <row r="13" spans="2:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F13" s="164" t="s">
         <v>253</v>
       </c>
@@ -13211,7 +13233,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F14" s="165" t="s">
         <v>254</v>
       </c>
@@ -13231,7 +13253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F15" s="166" t="s">
         <v>255</v>
       </c>
@@ -13251,7 +13273,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F16" s="167" t="s">
         <v>256</v>
       </c>
@@ -13271,7 +13293,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="17" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F17" s="168" t="s">
         <v>257</v>
       </c>
@@ -13291,7 +13313,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="18" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18" s="169" t="s">
         <v>258</v>
       </c>
@@ -13311,8 +13333,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
-    <row r="22" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="21" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F22" s="164"/>
       <c r="G22" s="163"/>
       <c r="H22" s="161"/>
@@ -13320,7 +13342,7 @@
       <c r="J22" s="161"/>
       <c r="K22" s="163"/>
     </row>
-    <row r="23" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="23" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F23" s="165"/>
       <c r="G23" s="162"/>
       <c r="H23" s="162"/>
@@ -13328,7 +13350,7 @@
       <c r="J23" s="162"/>
       <c r="K23" s="162"/>
     </row>
-    <row r="24" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="24" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F24" s="166"/>
       <c r="G24" s="162"/>
       <c r="H24" s="162"/>
@@ -13336,7 +13358,7 @@
       <c r="J24" s="162"/>
       <c r="K24" s="162"/>
     </row>
-    <row r="25" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="25" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F25" s="167"/>
       <c r="G25" s="162"/>
       <c r="H25" s="162"/>
@@ -13344,7 +13366,7 @@
       <c r="J25" s="162"/>
       <c r="K25" s="162"/>
     </row>
-    <row r="26" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="26" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F26" s="168"/>
       <c r="G26" s="162"/>
       <c r="H26" s="162"/>
@@ -13352,7 +13374,7 @@
       <c r="J26" s="162"/>
       <c r="K26" s="162"/>
     </row>
-    <row r="27" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="27" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F27" s="169"/>
       <c r="G27" s="162"/>
       <c r="H27" s="162"/>
@@ -13482,6 +13504,15 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </oddHeader>
+    <oddFooter xml:space="preserve">&amp;C      </oddFooter>
+    <evenHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </evenHeader>
+    <evenFooter xml:space="preserve">&amp;C      </evenFooter>
+    <firstHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </firstHeader>
+    <firstFooter xml:space="preserve">&amp;C      </firstFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -13493,12 +13524,12 @@
       <selection activeCell="E5" sqref="E5:F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:6" x14ac:dyDescent="0.75">
+    <row r="5" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>259</v>
       </c>
@@ -13506,7 +13537,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="5:6" x14ac:dyDescent="0.75">
+    <row r="6" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>273</v>
       </c>
@@ -13514,7 +13545,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="5:6" x14ac:dyDescent="0.75">
+    <row r="7" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>272</v>
       </c>
@@ -13522,7 +13553,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="8" spans="5:6" x14ac:dyDescent="0.75">
+    <row r="8" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>260</v>
       </c>
@@ -13530,7 +13561,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="9" spans="5:6" x14ac:dyDescent="0.75">
+    <row r="9" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>261</v>
       </c>
@@ -13538,7 +13569,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="5:6" x14ac:dyDescent="0.75">
+    <row r="10" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>262</v>
       </c>
@@ -13546,7 +13577,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="5:6" x14ac:dyDescent="0.75">
+    <row r="11" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>271</v>
       </c>
@@ -13554,7 +13585,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="5:6" x14ac:dyDescent="0.75">
+    <row r="12" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>263</v>
       </c>
@@ -13562,7 +13593,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="13" spans="5:6" x14ac:dyDescent="0.75">
+    <row r="13" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>264</v>
       </c>
@@ -13570,7 +13601,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="14" spans="5:6" x14ac:dyDescent="0.75">
+    <row r="14" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>265</v>
       </c>
@@ -13578,7 +13609,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="15" spans="5:6" x14ac:dyDescent="0.75">
+    <row r="15" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>266</v>
       </c>
@@ -13586,7 +13617,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="16" spans="5:6" x14ac:dyDescent="0.75">
+    <row r="16" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>270</v>
       </c>
@@ -13594,7 +13625,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.75">
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>267</v>
       </c>
@@ -13602,7 +13633,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.75">
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>268</v>
       </c>
@@ -13610,7 +13641,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.75">
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>269</v>
       </c>
@@ -13620,7 +13651,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </oddHeader>
+    <oddFooter xml:space="preserve">&amp;C      </oddFooter>
+    <evenHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </evenHeader>
+    <evenFooter xml:space="preserve">&amp;C      </evenFooter>
+    <firstHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </firstHeader>
+    <firstFooter xml:space="preserve">&amp;C      </firstFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -13632,17 +13672,17 @@
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.04296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.6796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.08984375" customWidth="1"/>
-    <col min="10" max="10" width="81.86328125" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="81.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="4" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E4" s="192" t="s">
         <v>274</v>
       </c>
@@ -13662,7 +13702,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="5" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E5" s="171"/>
       <c r="F5" s="56"/>
       <c r="G5" s="56"/>
@@ -13670,7 +13710,7 @@
       <c r="I5" s="56"/>
       <c r="J5" s="172"/>
     </row>
-    <row r="6" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="6" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E6" s="173" t="s">
         <v>148</v>
       </c>
@@ -13690,7 +13730,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="7" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="7" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E7" s="177"/>
       <c r="F7" s="178"/>
       <c r="G7" s="178"/>
@@ -13704,7 +13744,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="8" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="8" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E8" s="177"/>
       <c r="F8" s="178"/>
       <c r="G8" s="178"/>
@@ -13718,7 +13758,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="9" spans="5:10" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="9" spans="5:10" ht="30" x14ac:dyDescent="0.25">
       <c r="E9" s="177"/>
       <c r="F9" s="178"/>
       <c r="G9" s="178"/>
@@ -13732,7 +13772,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="10" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="10" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E10" s="177"/>
       <c r="F10" s="178"/>
       <c r="G10" s="178"/>
@@ -13746,7 +13786,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="11" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="11" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E11" s="177"/>
       <c r="F11" s="178"/>
       <c r="G11" s="178"/>
@@ -13760,7 +13800,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="12" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E12" s="177"/>
       <c r="F12" s="178"/>
       <c r="G12" s="178"/>
@@ -13774,7 +13814,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="13" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="13" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E13" s="177"/>
       <c r="F13" s="178"/>
       <c r="G13" s="178"/>
@@ -13788,7 +13828,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="14" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="14" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E14" s="177"/>
       <c r="F14" s="178"/>
       <c r="G14" s="178"/>
@@ -13802,7 +13842,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="15" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="15" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E15" s="177"/>
       <c r="F15" s="178"/>
       <c r="G15" s="178"/>
@@ -13816,7 +13856,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="16" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="16" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E16" s="182"/>
       <c r="F16" s="183"/>
       <c r="G16" s="183"/>
@@ -13824,7 +13864,7 @@
       <c r="I16" s="185"/>
       <c r="J16" s="186"/>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E17" s="173" t="s">
         <v>149</v>
       </c>
@@ -13844,7 +13884,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E18" s="187"/>
       <c r="F18" s="180"/>
       <c r="G18" s="180"/>
@@ -13858,7 +13898,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E19" s="187"/>
       <c r="F19" s="180"/>
       <c r="G19" s="180"/>
@@ -13872,7 +13912,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E20" s="187"/>
       <c r="F20" s="180"/>
       <c r="G20" s="180"/>
@@ -13886,7 +13926,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E21" s="187"/>
       <c r="F21" s="180"/>
       <c r="G21" s="180"/>
@@ -13900,7 +13940,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E22" s="187"/>
       <c r="F22" s="180"/>
       <c r="G22" s="180"/>
@@ -13914,7 +13954,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E23" s="187"/>
       <c r="F23" s="180"/>
       <c r="G23" s="180"/>
@@ -13928,7 +13968,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="24" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E24" s="187"/>
       <c r="F24" s="180"/>
       <c r="G24" s="180"/>
@@ -13942,7 +13982,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="25" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E25" s="187"/>
       <c r="F25" s="180"/>
       <c r="G25" s="180"/>
@@ -13956,7 +13996,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="26" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E26" s="187"/>
       <c r="F26" s="180"/>
       <c r="G26" s="180"/>
@@ -13970,7 +14010,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="27" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E27" s="187"/>
       <c r="F27" s="180"/>
       <c r="G27" s="180"/>
@@ -13984,7 +14024,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="28" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E28" s="187"/>
       <c r="F28" s="180"/>
       <c r="G28" s="180"/>
@@ -13998,7 +14038,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E29" s="187"/>
       <c r="F29" s="180"/>
       <c r="G29" s="180"/>
@@ -14012,7 +14052,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E30" s="187"/>
       <c r="F30" s="180"/>
       <c r="G30" s="180"/>
@@ -14026,7 +14066,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E31" s="188"/>
       <c r="F31" s="185"/>
       <c r="G31" s="185"/>
@@ -14034,7 +14074,7 @@
       <c r="I31" s="185"/>
       <c r="J31" s="186"/>
     </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E32" s="173" t="s">
         <v>152</v>
       </c>
@@ -14054,7 +14094,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E33" s="187"/>
       <c r="F33" s="180"/>
       <c r="G33" s="180"/>
@@ -14068,7 +14108,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E34" s="189"/>
       <c r="F34" s="185"/>
       <c r="G34" s="185"/>
@@ -14076,7 +14116,7 @@
       <c r="I34" s="185"/>
       <c r="J34" s="186"/>
     </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E35" s="173" t="s">
         <v>335</v>
       </c>
@@ -14096,7 +14136,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E36" s="187"/>
       <c r="F36" s="180"/>
       <c r="G36" s="180"/>
@@ -14110,7 +14150,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E37" s="188"/>
       <c r="F37" s="185"/>
       <c r="G37" s="185"/>
@@ -14118,7 +14158,7 @@
       <c r="I37" s="185"/>
       <c r="J37" s="186"/>
     </row>
-    <row r="38" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E38" s="173" t="s">
         <v>337</v>
       </c>
@@ -14138,7 +14178,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="39" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E39" s="187"/>
       <c r="F39" s="180"/>
       <c r="G39" s="180"/>
@@ -14152,7 +14192,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="40" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E40" s="188"/>
       <c r="F40" s="185"/>
       <c r="G40" s="185"/>
@@ -14160,7 +14200,7 @@
       <c r="I40" s="185"/>
       <c r="J40" s="186"/>
     </row>
-    <row r="41" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E41" s="173" t="s">
         <v>279</v>
       </c>
@@ -14180,7 +14220,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="42" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E42" s="188"/>
       <c r="F42" s="185"/>
       <c r="G42" s="185"/>
@@ -14188,7 +14228,7 @@
       <c r="I42" s="185"/>
       <c r="J42" s="186"/>
     </row>
-    <row r="43" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="43" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E43" s="173" t="s">
         <v>286</v>
       </c>
@@ -14208,7 +14248,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="44" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="44" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E44" s="188"/>
       <c r="F44" s="185"/>
       <c r="G44" s="185"/>
@@ -14216,7 +14256,7 @@
       <c r="I44" s="185"/>
       <c r="J44" s="186"/>
     </row>
-    <row r="45" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="45" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E45" s="173" t="s">
         <v>280</v>
       </c>
@@ -14236,7 +14276,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="46" spans="5:10" x14ac:dyDescent="0.75">
+    <row r="46" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E46" s="188"/>
       <c r="F46" s="185"/>
       <c r="G46" s="185"/>
@@ -14247,6 +14287,14 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </oddHeader>
+    <oddFooter xml:space="preserve">&amp;C      </oddFooter>
+    <evenHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </evenHeader>
+    <evenFooter xml:space="preserve">&amp;C      </evenFooter>
+    <firstHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </firstHeader>
+    <firstFooter xml:space="preserve">&amp;C      </firstFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -14261,15 +14309,15 @@
       <selection activeCell="E4" sqref="E4:H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.2265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" customWidth="1"/>
-    <col min="8" max="8" width="47.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="4" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E4" s="198" t="s">
         <v>340</v>
       </c>
@@ -14283,7 +14331,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="5" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="5" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E5" s="199">
         <v>43644</v>
       </c>
@@ -14297,7 +14345,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="6" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E6" s="199">
         <v>43665</v>
       </c>
@@ -14311,7 +14359,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="7" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E7" s="199">
         <v>43684</v>
       </c>
@@ -14325,7 +14373,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="8" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E8" s="199">
         <v>43690</v>
       </c>
@@ -14339,7 +14387,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="9" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E9" s="199">
         <v>43698</v>
       </c>
@@ -14353,7 +14401,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="10" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E10" s="199">
         <v>43703</v>
       </c>
@@ -14367,7 +14415,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="11" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="11" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E11" s="199">
         <v>43718</v>
       </c>
@@ -14381,7 +14429,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="12" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="12" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E12" s="199">
         <v>43739</v>
       </c>
@@ -14395,7 +14443,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="13" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E13" s="199">
         <v>43761</v>
       </c>
@@ -14409,7 +14457,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="14" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="14" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E14" s="199">
         <v>43784</v>
       </c>
@@ -14426,6 +14474,14 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </oddHeader>
+    <oddFooter xml:space="preserve">&amp;C      </oddFooter>
+    <evenHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </evenHeader>
+    <evenFooter xml:space="preserve">&amp;C      </evenFooter>
+    <firstHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </firstHeader>
+    <firstFooter xml:space="preserve">&amp;C      </firstFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -14440,14 +14496,14 @@
       <selection activeCell="E4" sqref="E4:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="6" width="10.2265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="4" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E4" s="198" t="s">
         <v>340</v>
       </c>
@@ -14461,7 +14517,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="5" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="5" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E5" s="201">
         <v>43640</v>
       </c>
@@ -14475,7 +14531,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="6" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E6" s="201">
         <v>43640</v>
       </c>
@@ -14489,7 +14545,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="7" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E7" s="201">
         <v>43640</v>
       </c>
@@ -14503,7 +14559,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="8" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E8" s="201">
         <v>43642</v>
       </c>
@@ -14517,7 +14573,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="9" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E9" s="201">
         <v>43642</v>
       </c>
@@ -14531,7 +14587,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="10" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="10" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E10" s="201">
         <v>43649</v>
       </c>
@@ -14545,7 +14601,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="11" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="11" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E11" s="201">
         <v>43655</v>
       </c>
@@ -14559,7 +14615,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="12" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="12" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E12" s="201">
         <v>43656</v>
       </c>
@@ -14573,7 +14629,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="13" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E13" s="201">
         <v>43656</v>
       </c>
@@ -14587,7 +14643,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="14" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="14" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E14" s="201">
         <v>43657</v>
       </c>
@@ -14601,7 +14657,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="15" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="15" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E15" s="201">
         <v>43663</v>
       </c>
@@ -14615,7 +14671,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="16" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="16" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E16" s="201">
         <v>43707</v>
       </c>
@@ -14629,7 +14685,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E17" s="201">
         <v>43697</v>
       </c>
@@ -14643,7 +14699,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E18" s="201">
         <v>43730</v>
       </c>
@@ -14657,7 +14713,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E19" s="201">
         <v>43735</v>
       </c>
@@ -14671,7 +14727,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E20" s="201">
         <v>43756</v>
       </c>
@@ -14685,7 +14741,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E21" s="201">
         <v>43768</v>
       </c>
@@ -14699,7 +14755,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E22" s="201">
         <v>43782</v>
       </c>
@@ -14713,7 +14769,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.75">
+    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E23" s="179" t="s">
         <v>396</v>
       </c>
@@ -14727,8 +14783,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </oddHeader>
+    <oddFooter xml:space="preserve">&amp;C      </oddFooter>
+    <evenHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </evenHeader>
+    <evenFooter xml:space="preserve">&amp;C      </evenFooter>
+    <firstHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </firstHeader>
+    <firstFooter xml:space="preserve">&amp;C      </firstFooter>
+  </headerFooter>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -14741,15 +14806,15 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="41.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="13.76953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.76953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
-    <row r="8" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="7" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F8" s="164" t="s">
         <v>253</v>
       </c>
@@ -14769,7 +14834,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="9" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="9" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F9" s="165" t="s">
         <v>254</v>
       </c>
@@ -14789,7 +14854,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="10" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="10" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" s="166" t="s">
         <v>255</v>
       </c>
@@ -14809,7 +14874,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="11" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="11" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F11" s="167" t="s">
         <v>256</v>
       </c>
@@ -14829,7 +14894,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="12" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="12" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F12" s="168" t="s">
         <v>257</v>
       </c>
@@ -14849,7 +14914,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="13" spans="6:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="13" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F13" s="169" t="s">
         <v>258</v>
       </c>
@@ -14891,23 +14956,38 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </oddHeader>
+    <oddFooter xml:space="preserve">&amp;C      </oddFooter>
+    <evenHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </evenHeader>
+    <evenFooter xml:space="preserve">&amp;C      </evenFooter>
+    <firstHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </firstHeader>
+    <firstFooter xml:space="preserve">&amp;C      </firstFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2E2C07E-0980-41C3-91D2-385E10BD1F71}">
-  <dimension ref="C3:F35"/>
+  <dimension ref="C3:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>442</v>
+      </c>
+      <c r="D3" t="s">
+        <v>441</v>
+      </c>
       <c r="E3" t="s">
         <v>439</v>
       </c>
@@ -14915,7 +14995,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C4" s="224" t="s">
         <v>427</v>
       </c>
@@ -14929,7 +15009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C5" s="224"/>
       <c r="D5" t="s">
         <v>431</v>
@@ -14941,7 +15021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" s="224"/>
       <c r="D6" t="s">
         <v>112</v>
@@ -14953,7 +15033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" s="224"/>
       <c r="D7" t="s">
         <v>118</v>
@@ -14965,7 +15045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" s="224"/>
       <c r="D8" t="s">
         <v>114</v>
@@ -14977,7 +15057,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" s="224"/>
       <c r="D9" t="s">
         <v>116</v>
@@ -14989,7 +15069,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" s="224"/>
       <c r="D10" t="s">
         <v>428</v>
@@ -15001,7 +15081,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" s="224"/>
       <c r="D11" t="s">
         <v>117</v>
@@ -15013,7 +15093,8 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="12" spans="3:6" s="225" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C13" s="224" t="s">
         <v>429</v>
       </c>
@@ -15027,7 +15108,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C14" s="224"/>
       <c r="D14" t="s">
         <v>124</v>
@@ -15039,7 +15120,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C15" s="224"/>
       <c r="D15" t="s">
         <v>127</v>
@@ -15051,7 +15132,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C16" s="224"/>
       <c r="D16" t="s">
         <v>432</v>
@@ -15063,7 +15144,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="224"/>
       <c r="D17" t="s">
         <v>126</v>
@@ -15075,7 +15156,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="224"/>
       <c r="D18" t="s">
         <v>121</v>
@@ -15087,7 +15168,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="224"/>
       <c r="D19" t="s">
         <v>125</v>
@@ -15099,7 +15180,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="224"/>
       <c r="D20" t="s">
         <v>433</v>
@@ -15111,7 +15192,8 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="21" spans="3:10" s="225" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="224" t="s">
         <v>434</v>
       </c>
@@ -15125,7 +15207,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="224"/>
       <c r="D23" t="s">
         <v>129</v>
@@ -15137,7 +15219,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="224"/>
       <c r="D24" t="s">
         <v>130</v>
@@ -15149,7 +15231,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="224"/>
       <c r="D25" t="s">
         <v>131</v>
@@ -15161,7 +15243,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="224"/>
       <c r="D26" t="s">
         <v>132</v>
@@ -15173,7 +15255,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="224"/>
       <c r="D27" t="s">
         <v>133</v>
@@ -15185,7 +15267,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="224"/>
       <c r="D28" t="s">
         <v>134</v>
@@ -15197,7 +15279,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" s="224"/>
       <c r="D29" t="s">
         <v>436</v>
@@ -15209,7 +15291,8 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="30" spans="3:10" s="225" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C31" s="224" t="s">
         <v>437</v>
       </c>
@@ -15222,8 +15305,9 @@
       <c r="F31" s="170">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.75">
+      <c r="J31" s="225"/>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C32" s="224"/>
       <c r="D32" t="s">
         <v>139</v>
@@ -15235,7 +15319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" s="224"/>
       <c r="D33" t="s">
         <v>136</v>
@@ -15247,7 +15331,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C34" s="224"/>
       <c r="D34" t="s">
         <v>137</v>
@@ -15259,7 +15343,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.75">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C35" s="224"/>
       <c r="D35" t="s">
         <v>438</v>
@@ -15279,17 +15363,20 @@
     <mergeCell ref="C31:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </oddHeader>
+    <oddFooter xml:space="preserve">&amp;C      </oddFooter>
+    <evenHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </evenHeader>
+    <evenFooter xml:space="preserve">&amp;C      </evenFooter>
+    <firstHeader xml:space="preserve">&amp;C&amp;"Arial,Regular"&amp;10     </firstHeader>
+    <firstFooter xml:space="preserve">&amp;C      </firstFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F33E8372F1A21F419469F20A538D343E" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="42a4145dfa7d4b5abf8c75a07cc1911b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3bf0cd4c-2448-4ff2-8213-a41beab8c9a9" xmlns:ns4="56e04384-c5e3-48db-802d-5469919b516a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d7a12eb2997e9a96616949852e8db7e8" ns3:_="" ns4:_="">
     <xsd:import namespace="3bf0cd4c-2448-4ff2-8213-a41beab8c9a9"/>
@@ -15460,6 +15547,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -15470,23 +15563,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA3192F1-D77C-4218-9B8F-6C8BC205D392}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="56e04384-c5e3-48db-802d-5469919b516a"/>
-    <ds:schemaRef ds:uri="3bf0cd4c-2448-4ff2-8213-a41beab8c9a9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10B5C290-ACB6-42AB-BF14-001193526EA0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15505,6 +15581,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA3192F1-D77C-4218-9B8F-6C8BC205D392}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="56e04384-c5e3-48db-802d-5469919b516a"/>
+    <ds:schemaRef ds:uri="3bf0cd4c-2448-4ff2-8213-a41beab8c9a9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6EE32A0-71F8-4E54-BFDA-6902525DD513}">
   <ds:schemaRefs>

</xml_diff>